<commit_message>
telah menambahkan banyak models beserta tabelnya, tinggal lanjut mencobanya
</commit_message>
<xml_diff>
--- a/skema-database.xlsx
+++ b/skema-database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ta-p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1554C8-C44B-4753-913D-D0EDAFDBE0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0393FD3-3BA2-4CB5-A96F-35A319313ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A57E6B4-B99A-443F-AC2E-63C9FAC4E642}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="81">
   <si>
     <t>Senin</t>
   </si>
@@ -62,47 +62,240 @@
     <t>Jadwal Mahasiswa</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>jadwal Dosen Dedy</t>
   </si>
   <si>
     <t>Dedy</t>
+  </si>
+  <si>
+    <t>jam</t>
+  </si>
+  <si>
+    <t>07.00-09.00</t>
+  </si>
+  <si>
+    <t>09.00-12.00</t>
+  </si>
+  <si>
+    <t>13.00-14.00</t>
+  </si>
+  <si>
+    <t>15.00-18.00</t>
+  </si>
+  <si>
+    <t>nama dosen</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>dedy</t>
+  </si>
+  <si>
+    <t>mina</t>
+  </si>
+  <si>
+    <t>ismu</t>
+  </si>
+  <si>
+    <t>tantra</t>
+  </si>
+  <si>
+    <t>rizky</t>
+  </si>
+  <si>
+    <t>nama mahasiswa</t>
+  </si>
+  <si>
+    <t>fan fan</t>
+  </si>
+  <si>
+    <t>angga</t>
+  </si>
+  <si>
+    <t>sidik</t>
+  </si>
+  <si>
+    <t>ocsa</t>
+  </si>
+  <si>
+    <t>program studi</t>
+  </si>
+  <si>
+    <t>sistem informasi</t>
+  </si>
+  <si>
+    <t>teknik informatika</t>
+  </si>
+  <si>
+    <t>matakuliah</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Pemrograman 4</t>
+  </si>
+  <si>
+    <t>Mp2</t>
+  </si>
+  <si>
+    <t>Bhs inggris</t>
+  </si>
+  <si>
+    <t>sks</t>
+  </si>
+  <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>program_studi_id</t>
+  </si>
+  <si>
+    <t>ruangan</t>
+  </si>
+  <si>
+    <t>ruang 21</t>
+  </si>
+  <si>
+    <t>ruang 10</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>kapasitas</t>
+  </si>
+  <si>
+    <t>kelas</t>
+  </si>
+  <si>
+    <t>kode matakuliah</t>
+  </si>
+  <si>
+    <t>JKW1234</t>
+  </si>
+  <si>
+    <t>RMN241</t>
+  </si>
+  <si>
+    <t>SND456</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>matakuliah_id</t>
+  </si>
+  <si>
+    <t>ruangan_id</t>
+  </si>
+  <si>
+    <t>reguler</t>
+  </si>
+  <si>
+    <t>sore</t>
+  </si>
+  <si>
+    <t>eksekutif</t>
+  </si>
+  <si>
+    <t>hari</t>
+  </si>
+  <si>
+    <t>senin</t>
+  </si>
+  <si>
+    <t>selasa</t>
+  </si>
+  <si>
+    <t>rabu</t>
+  </si>
+  <si>
+    <t>kamis</t>
+  </si>
+  <si>
+    <t>jumat</t>
+  </si>
+  <si>
+    <t>sabtu</t>
+  </si>
+  <si>
+    <t>minggu</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>dosen</t>
+  </si>
+  <si>
+    <t>mahasiswa</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fanfan</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>jadwal_dosen</t>
+  </si>
+  <si>
+    <t>hari_id</t>
+  </si>
+  <si>
+    <t>kelas_id</t>
+  </si>
+  <si>
+    <t>jam_pelajaran</t>
+  </si>
+  <si>
+    <t>jadwal_mahasiswa</t>
+  </si>
+  <si>
+    <t>jadwal_dosen_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -117,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,12 +318,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,20 +675,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6ACEE7-EAED-44A6-8349-90A6E25E94F8}">
-  <dimension ref="E15:K27"/>
+  <dimension ref="D15:AT48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="G14" workbookViewId="0">
+      <selection activeCell="AM38" sqref="AM38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="15" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="N15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="Q15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="5:21" x14ac:dyDescent="0.3">
+      <c r="N16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="Q16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="4:46" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>0</v>
       </c>
@@ -500,105 +778,257 @@
       <c r="K17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T17" s="1">
+        <v>123</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="4:46" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="1">
+        <v>2</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>2</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S18" s="1">
+        <v>12228416</v>
+      </c>
+      <c r="T18" s="1">
+        <v>123</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="1">
+        <v>3</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>3</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S19" s="1">
+        <v>1231261</v>
+      </c>
+      <c r="T19" s="1">
+        <v>123</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" s="1">
+        <v>4</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+    </row>
+    <row r="21" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" s="1"/>
+      <c r="T21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="AA21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AE21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AL21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM21" s="1"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+    </row>
+    <row r="22" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="N22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AL22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+    </row>
+    <row r="23" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="N23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T23" s="1">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X23" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>20</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AL23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS23" s="1"/>
+      <c r="AT23" s="1"/>
+    </row>
+    <row r="24" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
         <v>10</v>
       </c>
-      <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>0</v>
       </c>
@@ -620,26 +1050,342 @@
       <c r="K24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>2</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T24" s="1">
+        <v>2</v>
+      </c>
+      <c r="U24" s="1">
+        <v>2</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X24" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>20</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AL24" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+    </row>
+    <row r="25" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
       <c r="E25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T25" s="1">
+        <v>3</v>
+      </c>
+      <c r="U25" s="1">
+        <v>1</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X25" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>50</v>
+      </c>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AL25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+    </row>
+    <row r="26" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
       <c r="H26" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="K26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="N26" s="1">
+        <v>3</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AL26" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS26" s="1"/>
+      <c r="AT26" s="1"/>
+    </row>
+    <row r="27" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
       <c r="G27" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="N27" s="1">
+        <v>4</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AL27" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM27" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="1">
+        <v>5</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL28" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM28" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="AL29" s="1">
+        <v>7</v>
+      </c>
+      <c r="AM29" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF36" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM36" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF37">
+        <v>1</v>
+      </c>
+      <c r="AG37">
+        <v>3</v>
+      </c>
+      <c r="AH37">
+        <v>1</v>
+      </c>
+      <c r="AI37">
+        <v>2</v>
+      </c>
+      <c r="AJ37">
+        <v>3</v>
+      </c>
+      <c r="AK37">
+        <v>1</v>
+      </c>
+      <c r="AL37">
+        <v>1</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF38">
+        <v>2</v>
+      </c>
+      <c r="AG38">
+        <v>2</v>
+      </c>
+      <c r="AH38">
+        <v>2</v>
+      </c>
+      <c r="AI38">
+        <v>2</v>
+      </c>
+      <c r="AJ38">
+        <v>3</v>
+      </c>
+      <c r="AK38">
+        <v>3</v>
+      </c>
+      <c r="AL38">
+        <v>1</v>
+      </c>
+      <c r="AM38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF39">
+        <v>3</v>
+      </c>
+      <c r="AL39">
+        <v>1</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF40">
+        <v>4</v>
+      </c>
+      <c r="AL40">
+        <v>2</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF47">
+        <v>1</v>
+      </c>
+      <c r="AG47">
+        <v>1</v>
+      </c>
+      <c r="AH47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="32:39" x14ac:dyDescent="0.3">
+      <c r="AF48">
+        <v>2</v>
+      </c>
+      <c r="AG48">
+        <v>1</v>
+      </c>
+      <c r="AH48">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Menganti Relasi yang sebelumnya dan telah mengeceknya baru hanya sampai jadwal
</commit_message>
<xml_diff>
--- a/skema-database.xlsx
+++ b/skema-database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ta-p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0393FD3-3BA2-4CB5-A96F-35A319313ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFB26C8-7F5F-488F-886B-04DD316FC167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A57E6B4-B99A-443F-AC2E-63C9FAC4E642}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>Senin</t>
   </si>
@@ -89,9 +89,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>nama</t>
-  </si>
-  <si>
     <t>dedy</t>
   </si>
   <si>
@@ -107,21 +104,6 @@
     <t>rizky</t>
   </si>
   <si>
-    <t>nama mahasiswa</t>
-  </si>
-  <si>
-    <t>fan fan</t>
-  </si>
-  <si>
-    <t>angga</t>
-  </si>
-  <si>
-    <t>sidik</t>
-  </si>
-  <si>
-    <t>ocsa</t>
-  </si>
-  <si>
     <t>program studi</t>
   </si>
   <si>
@@ -188,97 +170,100 @@
     <t>user_id</t>
   </si>
   <si>
+    <t>reguler</t>
+  </si>
+  <si>
+    <t>sore</t>
+  </si>
+  <si>
+    <t>eksekutif</t>
+  </si>
+  <si>
+    <t>hari</t>
+  </si>
+  <si>
+    <t>senin</t>
+  </si>
+  <si>
+    <t>selasa</t>
+  </si>
+  <si>
+    <t>rabu</t>
+  </si>
+  <si>
+    <t>kamis</t>
+  </si>
+  <si>
+    <t>jumat</t>
+  </si>
+  <si>
+    <t>sabtu</t>
+  </si>
+  <si>
+    <t>minggu</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>dosen</t>
+  </si>
+  <si>
+    <t>mahasiswa</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fanfan</t>
+  </si>
+  <si>
+    <t>jadwal_kuliah</t>
+  </si>
+  <si>
+    <t>nama_dosen_id</t>
+  </si>
+  <si>
+    <t>PRB222</t>
+  </si>
+  <si>
+    <t>Analisis Data</t>
+  </si>
+  <si>
+    <t>jam_ke</t>
+  </si>
+  <si>
+    <t>user_jadwal_kuliah_table</t>
+  </si>
+  <si>
+    <t>19:00-21:00</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>pivot many to many</t>
+  </si>
+  <si>
     <t>matakuliah_id</t>
   </si>
   <si>
     <t>ruangan_id</t>
   </si>
   <si>
-    <t>reguler</t>
-  </si>
-  <si>
-    <t>sore</t>
-  </si>
-  <si>
-    <t>eksekutif</t>
-  </si>
-  <si>
-    <t>hari</t>
-  </si>
-  <si>
-    <t>senin</t>
-  </si>
-  <si>
-    <t>selasa</t>
-  </si>
-  <si>
-    <t>rabu</t>
-  </si>
-  <si>
-    <t>kamis</t>
-  </si>
-  <si>
-    <t>jumat</t>
-  </si>
-  <si>
-    <t>sabtu</t>
-  </si>
-  <si>
-    <t>minggu</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>dosen</t>
-  </si>
-  <si>
-    <t>mahasiswa</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>fanfan</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>jadwal_dosen</t>
-  </si>
-  <si>
     <t>hari_id</t>
   </si>
   <si>
     <t>kelas_id</t>
-  </si>
-  <si>
-    <t>jam_pelajaran</t>
-  </si>
-  <si>
-    <t>jadwal_mahasiswa</t>
-  </si>
-  <si>
-    <t>jadwal_dosen_id</t>
   </si>
 </sst>
 </file>
@@ -337,10 +322,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6ACEE7-EAED-44A6-8349-90A6E25E94F8}">
-  <dimension ref="D15:AT48"/>
+  <dimension ref="D15:AT47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G14" workbookViewId="0">
-      <selection activeCell="AM38" sqref="AM38"/>
+    <sheetView tabSelected="1" topLeftCell="O17" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AK36" sqref="AK36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,16 +679,17 @@
     <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.88671875" customWidth="1"/>
     <col min="28" max="28" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="5.21875" bestFit="1" customWidth="1"/>
@@ -710,7 +697,7 @@
     <col min="33" max="33" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11.88671875" bestFit="1" customWidth="1"/>
@@ -723,12 +710,10 @@
       <c r="E15" t="s">
         <v>7</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="Q15" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -736,24 +721,22 @@
       <c r="U15" s="1"/>
     </row>
     <row r="16" spans="5:21" x14ac:dyDescent="0.3">
-      <c r="N16" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="Q16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="4:46" x14ac:dyDescent="0.3">
@@ -778,43 +761,35 @@
       <c r="K17" t="s">
         <v>6</v>
       </c>
-      <c r="N17" s="1">
-        <v>1</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
       <c r="Q17" s="1">
         <v>1</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="T17" s="1">
         <v>123</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="4:46" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="N18" s="1">
-        <v>2</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
       <c r="Q18" s="1">
         <v>2</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="S18" s="1">
         <v>12228416</v>
@@ -823,24 +798,20 @@
         <v>123</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="4:46" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="1">
-        <v>3</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
       <c r="Q19" s="1">
         <v>3</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S19" s="1">
         <v>1231261</v>
@@ -849,21 +820,17 @@
         <v>123</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="4:46" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
-        <v>20</v>
-      </c>
-      <c r="N20" s="1">
-        <v>4</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
       <c r="AE20" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
@@ -873,22 +840,14 @@
     </row>
     <row r="21" spans="4:46" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="T21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
       <c r="AA21" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
@@ -896,13 +855,13 @@
         <v>16</v>
       </c>
       <c r="AF21" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AL21" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="AM21" s="1"/>
       <c r="AS21" s="1"/>
@@ -917,40 +876,22 @@
         <v>16</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="AE22" s="1">
         <v>1</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
@@ -959,7 +900,7 @@
         <v>16</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="AS22" s="1"/>
       <c r="AT22" s="1"/>
@@ -972,37 +913,19 @@
         <v>16</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="Q23" s="1">
         <v>1</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T23" s="1">
-        <v>1</v>
-      </c>
-      <c r="U23" s="1">
-        <v>1</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X23" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y23" s="1">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="AA23" s="1">
         <v>1</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="AC23" s="1">
         <v>20</v>
@@ -1011,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="AF23" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
@@ -1020,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="AM23" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="AS23" s="1"/>
       <c r="AT23" s="1"/>
@@ -1054,37 +977,19 @@
         <v>1</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="Q24" s="1">
         <v>2</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T24" s="1">
-        <v>2</v>
-      </c>
-      <c r="U24" s="1">
-        <v>2</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X24" s="1">
-        <v>3</v>
-      </c>
-      <c r="Y24" s="1">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="AA24" s="1">
         <v>2</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="AC24" s="1">
         <v>20</v>
@@ -1093,7 +998,7 @@
         <v>3</v>
       </c>
       <c r="AF24" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
@@ -1102,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="AM24" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="AS24" s="1"/>
       <c r="AT24" s="1"/>
@@ -1118,31 +1023,13 @@
         <v>2</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T25" s="1">
-        <v>3</v>
-      </c>
-      <c r="U25" s="1">
-        <v>1</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X25" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y25" s="1">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="AA25" s="1">
         <v>3</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="AC25" s="1">
         <v>50</v>
@@ -1156,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="AM25" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="AS25" s="1"/>
       <c r="AT25" s="1"/>
@@ -1175,7 +1062,10 @@
         <v>3</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="T26" t="s">
+        <v>71</v>
       </c>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
@@ -1186,7 +1076,7 @@
         <v>4</v>
       </c>
       <c r="AM26" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AS26" s="1"/>
       <c r="AT26" s="1"/>
@@ -1202,8 +1092,17 @@
         <v>4</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
@@ -1213,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="AM27" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="4:46" x14ac:dyDescent="0.3">
@@ -1224,165 +1123,299 @@
         <v>5</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="AL28" s="1">
         <v>6</v>
       </c>
       <c r="AM28" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="T29" s="1">
+        <v>1</v>
+      </c>
+      <c r="U29" s="1">
+        <v>1</v>
+      </c>
+      <c r="V29" s="1">
+        <v>1</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>2</v>
+      </c>
       <c r="AL29" s="1">
         <v>7</v>
       </c>
       <c r="AM29" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="T30" s="1">
+        <v>2</v>
+      </c>
+      <c r="U30" s="1">
+        <v>1</v>
+      </c>
+      <c r="V30" s="1">
+        <v>2</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="T31" s="1">
+        <v>3</v>
+      </c>
+      <c r="U31" s="1">
+        <v>2</v>
+      </c>
+      <c r="V31" s="1">
+        <v>1</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="4:46" x14ac:dyDescent="0.3">
+      <c r="T32" s="2">
+        <v>4</v>
+      </c>
+      <c r="U32" s="1">
+        <v>2</v>
+      </c>
+      <c r="V32" s="2">
+        <v>2</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y32" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="AF34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="AF35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="1"/>
+      <c r="AK35" s="1"/>
+    </row>
+    <row r="36" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="AF36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ36" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF36" t="s">
+      <c r="AK36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="AF37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH37" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI37" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ37" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK37" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="AF38" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+    </row>
+    <row r="39" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y39" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF39" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+    </row>
+    <row r="40" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AF40" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG40" s="1"/>
+      <c r="AH40" s="1"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
+      <c r="AK40" s="1"/>
+    </row>
+    <row r="41" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AG36" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH36" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI36" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK36" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL36" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM36" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF37">
-        <v>1</v>
-      </c>
-      <c r="AG37">
-        <v>3</v>
-      </c>
-      <c r="AH37">
-        <v>1</v>
-      </c>
-      <c r="AI37">
-        <v>2</v>
-      </c>
-      <c r="AJ37">
-        <v>3</v>
-      </c>
-      <c r="AK37">
-        <v>1</v>
-      </c>
-      <c r="AL37">
-        <v>1</v>
-      </c>
-      <c r="AM37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF38">
-        <v>2</v>
-      </c>
-      <c r="AG38">
-        <v>2</v>
-      </c>
-      <c r="AH38">
-        <v>2</v>
-      </c>
-      <c r="AI38">
-        <v>2</v>
-      </c>
-      <c r="AJ38">
-        <v>3</v>
-      </c>
-      <c r="AK38">
-        <v>3</v>
-      </c>
-      <c r="AL38">
-        <v>1</v>
-      </c>
-      <c r="AM38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF39">
-        <v>3</v>
-      </c>
-      <c r="AL39">
-        <v>1</v>
-      </c>
-      <c r="AM39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF40">
+      <c r="Z41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF41" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" s="1"/>
+      <c r="AJ41" s="1"/>
+      <c r="AK41" s="1"/>
+    </row>
+    <row r="42" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y42" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y43" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y44" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y45" s="1">
         <v>4</v>
       </c>
-      <c r="AL40">
-        <v>2</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF45" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG46" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF47">
-        <v>1</v>
-      </c>
-      <c r="AG47">
-        <v>1</v>
-      </c>
-      <c r="AH47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="32:39" x14ac:dyDescent="0.3">
-      <c r="AF48">
-        <v>2</v>
-      </c>
-      <c r="AG48">
-        <v>1</v>
-      </c>
-      <c r="AH48">
-        <v>2</v>
-      </c>
+      <c r="Z45" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1"/>
+    </row>
+    <row r="47" spans="25:37" x14ac:dyDescent="0.3">
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>